<commit_message>
Video og datasett i kap 6
</commit_message>
<xml_diff>
--- a/seriediagram.xlsx
+++ b/seriediagram.xlsx
@@ -1,21 +1,45 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uinnlandet-my.sharepoint.com/personal/nils_kvilvang_inn_no/Documents/Undervisning/SPC_book/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="10" documentId="11_2C7AFDCE8F79A8D366075C52F36672F2725DD74D" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8BD75001-10BB-46AF-B65F-9B6C9A396BA9}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>value</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,11 +87,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -109,7 +141,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -141,9 +173,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -175,6 +225,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -350,138 +418,138 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A25"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>value</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
+    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>16.79301317129912</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>16.793013171299119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>16.52225126382552</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>17.74622224118976</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>17.746222241189759</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>14.72866387698602</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>14.728663876986021</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>18.19738953255477</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>18.197389532554769</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>16.43313077709198</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>16.433130777091979</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>14.42980036951461</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>14.429800369514609</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>15.06509433292393</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>16.06349334525979</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>15.99760666381899</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>13.72321875975337</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>13.723218759753371</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>16.75741222512548</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>16.757412225125481</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>15.45159444597197</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>15.451594445971971</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>16.17254947785038</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>16.172549477850382</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>16.56285306775542</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>17.51181795943768</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>17.511817959437678</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>16.65902516916441</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>16.659025169164408</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17.12202807467456</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>15.21535863085354</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>15.57430771118969</v>
-      </c>
-    </row>
-    <row r="22">
+        <v>15.574307711189689</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>16.39299759137217</v>
-      </c>
-    </row>
-    <row r="23">
+        <v>16.392997591372168</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>16.03675712982456</v>
-      </c>
-    </row>
-    <row r="24">
+        <v>16.036757129824561</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>14.96791633877171</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>14.73513852861858</v>
+        <v>14.735138528618579</v>
       </c>
     </row>
   </sheetData>

</xml_diff>